<commit_message>
coat-588 의 index 및 ruid의 오타수정
588 -> 411으로 변경
</commit_message>
<xml_diff>
--- a/table/item.xlsx
+++ b/table/item.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\MScannot206Server\table\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\MScannot206\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE14F19-5608-47A1-9088-D8BFCE809E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD8C976-E6E2-47E2-9CF7-E2D72321C473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BE16A6F-FF36-4601-894B-FA43EFA090D5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2BE16A6F-FF36-4601-894B-FA43EFA090D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2479" uniqueCount="1845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2479" uniqueCount="1847">
   <si>
     <t>Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -7370,6 +7370,14 @@
   </si>
   <si>
     <t>body</t>
+  </si>
+  <si>
+    <t>coat-411</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a1e00ed180704baca0c41faa6a595491</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -7850,10 +7858,10 @@
   <dimension ref="A1:E619"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B565" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C607" sqref="C607"/>
+      <selection pane="bottomRight" activeCell="E184" sqref="E184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -10438,7 +10446,7 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="4" t="s">
-        <v>512</v>
+        <v>1845</v>
       </c>
       <c r="B184" s="4" t="s">
         <v>518</v>
@@ -10447,7 +10455,7 @@
         <v>482</v>
       </c>
       <c r="E184" s="4" t="s">
-        <v>543</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>